<commit_message>
some changes in admin.py and exam scores excel file
</commit_message>
<xml_diff>
--- a/disciplines/exam_scores_new.xlsx
+++ b/disciplines/exam_scores_new.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\djprojects\umo\disciplines\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\inetpub\umo\disciplines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F968CE0-3A43-4035-8A9F-2E0C279067A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Лист 1" sheetId="1" r:id="rId1"/>
@@ -135,31 +134,14 @@
     <t>F</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Директор ИМИ СВФУ____________________ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>В. И. Афанасьева</t>
-    </r>
+    <t>Директор ИМИ СВФУ____________________ Н.Р. Пинигина</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -171,12 +153,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -240,23 +216,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -570,14 +546,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:ALZ24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -596,381 +572,381 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
       <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
       <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:10" ht="99.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:10" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="5" t="s">
         <v>11</v>
       </c>
       <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
       <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
       <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="7" t="s">
+      <c r="A14" s="4"/>
+      <c r="B14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>0</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="10" t="s">
+      <c r="D14" s="4"/>
+      <c r="E14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10" t="s">
+      <c r="F14" s="8"/>
+      <c r="G14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
       <c r="J14" s="3"/>
     </row>
     <row r="15" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="7" t="s">
+      <c r="A15" s="4"/>
+      <c r="B15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>0</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="7" t="s">
+      <c r="D15" s="4"/>
+      <c r="E15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7" t="s">
+      <c r="F15" s="6"/>
+      <c r="G15" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
       <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="7" t="s">
+      <c r="A16" s="4"/>
+      <c r="B16" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>0</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="7" t="s">
+      <c r="D16" s="4"/>
+      <c r="E16" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7" t="s">
+      <c r="F16" s="6"/>
+      <c r="G16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
       <c r="J16" s="3"/>
     </row>
     <row r="17" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="7" t="s">
+      <c r="A17" s="4"/>
+      <c r="B17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <v>0</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="7" t="s">
+      <c r="D17" s="4"/>
+      <c r="E17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7" t="s">
+      <c r="F17" s="6"/>
+      <c r="G17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
       <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="B18" s="7" t="s">
+      <c r="A18" s="4"/>
+      <c r="B18" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="6">
         <v>0</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="7" t="s">
+      <c r="D18" s="4"/>
+      <c r="E18" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7" t="s">
+      <c r="F18" s="6"/>
+      <c r="G18" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
       <c r="J18" s="3"/>
     </row>
     <row r="19" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
-      <c r="B19" s="7" t="s">
+      <c r="A19" s="4"/>
+      <c r="B19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="6">
         <v>0</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="7" t="s">
+      <c r="D19" s="4"/>
+      <c r="E19" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7" t="s">
+      <c r="F19" s="6"/>
+      <c r="G19" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
       <c r="J19" s="3"/>
     </row>
     <row r="20" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" s="7" t="s">
+      <c r="A20" s="4"/>
+      <c r="B20" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="6">
         <v>0</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="7" t="s">
+      <c r="D20" s="4"/>
+      <c r="E20" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7" t="s">
+      <c r="F20" s="6"/>
+      <c r="G20" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
       <c r="J20" s="3"/>
     </row>
     <row r="21" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
-      <c r="B21" s="7" t="s">
+      <c r="A21" s="4"/>
+      <c r="B21" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <v>0</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="7" t="s">
+      <c r="D21" s="4"/>
+      <c r="E21" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7" t="s">
+      <c r="F21" s="6"/>
+      <c r="G21" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
       <c r="J21" s="3"/>
     </row>
     <row r="22" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
       <c r="J22" s="3"/>
     </row>
     <row r="23" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+    <row r="24" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
       <c r="J24" s="2"/>
     </row>
   </sheetData>

</xml_diff>